<commit_message>
Updated and merged HW2Q3a
</commit_message>
<xml_diff>
--- a/project/Sprint04.xlsx
+++ b/project/Sprint04.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" tabRatio="725"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" tabRatio="725"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -529,19 +529,19 @@
                   <c:v>39.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39.5</c:v>
+                  <c:v>42.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1763,7 +1763,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G10" sqref="G10:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,36 +1830,36 @@
         <v>3</v>
       </c>
       <c r="D2" s="24">
-        <f>SUM(D$4:D$995)</f>
+        <f t="shared" ref="D2:K2" si="0">SUM(D$4:D$995)</f>
         <v>39.5</v>
       </c>
       <c r="E2" s="25">
-        <f>SUM(E$4:E$995)</f>
+        <f t="shared" si="0"/>
         <v>39.5</v>
       </c>
       <c r="F2" s="25">
-        <f>SUM(F$4:F$995)</f>
+        <f t="shared" si="0"/>
         <v>39.5</v>
       </c>
       <c r="G2" s="25">
-        <f>SUM(G$4:G$995)</f>
-        <v>39.5</v>
+        <f t="shared" si="0"/>
+        <v>42.5</v>
       </c>
       <c r="H2" s="25">
-        <f>SUM(H$4:H$995)</f>
-        <v>39.5</v>
+        <f t="shared" si="0"/>
+        <v>42.5</v>
       </c>
       <c r="I2" s="25">
-        <f>SUM(I$4:I$995)</f>
-        <v>39.5</v>
+        <f t="shared" si="0"/>
+        <v>42.5</v>
       </c>
       <c r="J2" s="25">
-        <f>SUM(J$4:J$995)</f>
-        <v>39.5</v>
+        <f t="shared" si="0"/>
+        <v>42.5</v>
       </c>
       <c r="K2" s="25">
-        <f>SUM(K$4:K$995)</f>
-        <v>39.5</v>
+        <f t="shared" si="0"/>
+        <v>42.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1873,31 +1873,31 @@
         <v>39.5</v>
       </c>
       <c r="E3" s="25">
-        <f t="shared" ref="E3:K3" si="0">D$3-$D$2/7</f>
+        <f t="shared" ref="E3:K3" si="1">D$3-$D$2/7</f>
         <v>33.857142857142854</v>
       </c>
       <c r="F3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28.214285714285712</v>
       </c>
       <c r="G3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.571428571428569</v>
       </c>
       <c r="H3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.928571428571427</v>
       </c>
       <c r="I3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.285714285714285</v>
       </c>
       <c r="J3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.6428571428571415</v>
       </c>
       <c r="K3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L3" s="6" t="s">
@@ -1922,27 +1922,27 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:K13" si="1">E4</f>
+        <f t="shared" ref="F4:K13" si="2">E4</f>
         <v>2</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L4" t="s">
@@ -1967,31 +1967,31 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:K13" si="2">D5</f>
+        <f t="shared" ref="E5:E13" si="3">D5</f>
         <v>2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L5" t="s">
@@ -2016,31 +2016,31 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="L6" t="s">
@@ -2065,31 +2065,31 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2107,31 +2107,31 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:E9" si="3">D8</f>
+        <f t="shared" ref="E8:E9" si="4">D8</f>
         <v>1</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2149,31 +2149,31 @@
         <v>0.5</v>
       </c>
       <c r="E9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="J9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2191,32 +2191,31 @@
         <v>10</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="J10">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2233,32 +2232,31 @@
         <v>10</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="J11">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2275,32 +2273,31 @@
         <v>10</v>
       </c>
       <c r="E12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="J12">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2317,31 +2314,31 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
HW2 'done' to the point that a few questions are impossible Updated sprint4 document to reflect the pain of HW2
</commit_message>
<xml_diff>
--- a/project/Sprint04.xlsx
+++ b/project/Sprint04.xlsx
@@ -143,7 +143,8 @@
     <t>Continuing work on HW2
 HW2 is larger than initially planned by an order of magnitude
 Paper selection finalized, going to start making notes and doing supplemental research
-Project is on hold until other work is done</t>
+Project is on hold until other work is done
+HW2 ended up taking a total of 60+ man-hours of effort from the team, we essentially canceled all other work for the iteration</t>
   </si>
 </sst>
 </file>
@@ -294,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -358,10 +359,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,10 +538,10 @@
                   <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1760,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:G12"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1855,11 +1855,11 @@
       </c>
       <c r="J2" s="25">
         <f t="shared" si="0"/>
-        <v>42.5</v>
+        <v>12.5</v>
       </c>
       <c r="K2" s="25">
         <f t="shared" si="0"/>
-        <v>42.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2210,12 +2210,11 @@
         <v>11</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2251,12 +2250,11 @@
         <v>11</v>
       </c>
       <c r="J11">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2292,12 +2290,11 @@
         <v>11</v>
       </c>
       <c r="J12">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2342,50 +2339,119 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:B3"/>
-    <mergeCell ref="A14:E18"/>
+    <mergeCell ref="A14:K21"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19 C4:C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C13">
       <formula1>"Peter, Daniela, Jennifer"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>